<commit_message>
Designing the template structure for the complex report
</commit_message>
<xml_diff>
--- a/src/test/resources/complex/Complex_Translated.xlsx
+++ b/src/test/resources/complex/Complex_Translated.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fwhkp002vf\cal\home\Desktop\hackathon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesusdayo/Documents/json-excel/src/test/resources/complex/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7D9DC3-9C84-4D4D-9FA2-275B587D7428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="0" windowWidth="16395" windowHeight="6270" activeTab="2"/>
+    <workbookView xWindow="1320" yWindow="500" windowWidth="17200" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pension Investment Status" sheetId="3" r:id="rId1"/>
@@ -19,7 +20,19 @@
   <definedNames>
     <definedName name="EQPosnDate">'Stock Balance'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -383,7 +396,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0_ "/>
@@ -1762,6 +1775,60 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="6" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1786,9 +1853,6 @@
     <xf numFmtId="38" fontId="2" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="38" fontId="2" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1798,63 +1862,39 @@
     <xf numFmtId="38" fontId="2" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="28" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="29" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="22" fillId="0" borderId="6" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="41" fillId="38" borderId="30" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="41" fillId="38" borderId="31" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="41" fillId="38" borderId="32" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="40" fontId="22" fillId="0" borderId="30" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1864,36 +1904,9 @@
     <xf numFmtId="40" fontId="22" fillId="0" borderId="32" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="28" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="29" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="41" fillId="38" borderId="30" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="41" fillId="38" borderId="31" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="41" fillId="38" borderId="32" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="88">
-    <cellStyle name="_株式業種別要因分析" xfId="1"/>
+    <cellStyle name="_株式業種別要因分析" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="4" builtinId="38" customBuiltin="1"/>
@@ -1919,68 +1932,68 @@
     <cellStyle name="Accent5" xfId="24" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="25" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="26" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Bad 2" xfId="27"/>
+    <cellStyle name="Bad 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
     <cellStyle name="Calculation" xfId="28" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="29" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Comma" xfId="30" builtinId="3"/>
-    <cellStyle name="Comma [0] 2" xfId="31"/>
-    <cellStyle name="Comma 2" xfId="32"/>
-    <cellStyle name="Comma 2 2" xfId="33"/>
-    <cellStyle name="Comma 2 2 2" xfId="34"/>
-    <cellStyle name="Comma 2 3" xfId="35"/>
-    <cellStyle name="Comma 2 4" xfId="36"/>
-    <cellStyle name="Comma 3" xfId="37"/>
-    <cellStyle name="Comma 3 2" xfId="38"/>
-    <cellStyle name="Comma 4" xfId="39"/>
-    <cellStyle name="Comma 5" xfId="40"/>
-    <cellStyle name="Comma 5 2" xfId="41"/>
-    <cellStyle name="Comma 5 3" xfId="42"/>
-    <cellStyle name="Comma 6" xfId="43"/>
+    <cellStyle name="Comma [0] 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Comma 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Comma 2 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Comma 2 2 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Comma 2 3" xfId="35" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Comma 2 4" xfId="36" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Comma 3" xfId="37" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Comma 3 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Comma 4" xfId="39" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Comma 5" xfId="40" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Comma 5 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Comma 5 3" xfId="42" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Comma 6" xfId="43" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
     <cellStyle name="Explanatory Text" xfId="44" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="45" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Good 2" xfId="46"/>
-    <cellStyle name="Good 2 2" xfId="47"/>
+    <cellStyle name="Good 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Good 2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
     <cellStyle name="Heading 1" xfId="48" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="49" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="50" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="51" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink 2" xfId="52"/>
-    <cellStyle name="Hyperlink 3" xfId="53"/>
-    <cellStyle name="Hyperlink 4" xfId="54"/>
+    <cellStyle name="Hyperlink 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Hyperlink 3" xfId="53" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Hyperlink 4" xfId="54" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
     <cellStyle name="Input" xfId="55" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="56" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="57" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Neutral 2" xfId="58"/>
-    <cellStyle name="Neutral 2 2" xfId="59"/>
+    <cellStyle name="Neutral 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Neutral 2 2" xfId="59" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="60"/>
-    <cellStyle name="Normal 2 2" xfId="61"/>
-    <cellStyle name="Normal 2 2 2" xfId="62"/>
-    <cellStyle name="Normal 2 2 3" xfId="63"/>
-    <cellStyle name="Normal 2 3" xfId="64"/>
-    <cellStyle name="Normal 2 3 2" xfId="65"/>
-    <cellStyle name="Normal 2 4" xfId="66"/>
-    <cellStyle name="Normal 2 5" xfId="67"/>
-    <cellStyle name="Normal 3" xfId="68"/>
-    <cellStyle name="Normal 3 2" xfId="69"/>
-    <cellStyle name="Normal 3 2 2" xfId="70"/>
-    <cellStyle name="Normal 4" xfId="71"/>
-    <cellStyle name="Normal 4 2" xfId="72"/>
-    <cellStyle name="Normal 5" xfId="73"/>
-    <cellStyle name="Normal 6" xfId="74"/>
-    <cellStyle name="Normal 6 2" xfId="75"/>
-    <cellStyle name="Normal 6 3" xfId="76"/>
-    <cellStyle name="Normal 7" xfId="77"/>
-    <cellStyle name="Normal 8" xfId="78"/>
-    <cellStyle name="Normal 9" xfId="79"/>
+    <cellStyle name="Normal 2" xfId="60" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Normal 2 2" xfId="61" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Normal 2 2 3" xfId="63" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Normal 2 3" xfId="64" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Normal 2 3 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Normal 2 4" xfId="66" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Normal 2 5" xfId="67" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Normal 3" xfId="68" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal 3 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Normal 4" xfId="71" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Normal 4 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Normal 5" xfId="73" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Normal 6" xfId="74" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 6 2" xfId="75" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 6 3" xfId="76" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 7" xfId="77" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 8" xfId="78" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 9" xfId="79" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
     <cellStyle name="Note" xfId="80" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="81" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent 2" xfId="82"/>
+    <cellStyle name="Percent 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
     <cellStyle name="Title" xfId="83" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="84" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="85" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="卨げ" xfId="86"/>
-    <cellStyle name="湪" xfId="87"/>
+    <cellStyle name="卨げ" xfId="86" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="湪" xfId="87" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2007,7 +2020,13 @@
     <xdr:ext cx="0" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="114" name="worksheetKey" descr="{&quot;key&quot;:&quot;worksheetKey&quot;,&quot;value&quot;:&quot;3e60022c-3e82-4c40-b7c5-069ceb62abcf&quot;}" hidden="1"/>
+        <xdr:cNvPr id="114" name="worksheetKey" descr="{&quot;key&quot;:&quot;worksheetKey&quot;,&quot;value&quot;:&quot;3e60022c-3e82-4c40-b7c5-069ceb62abcf&quot;}" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000072000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2064,7 +2083,13 @@
     <xdr:ext cx="0" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="116" name="worksheetKey" descr="{&quot;key&quot;:&quot;worksheetKey&quot;,&quot;value&quot;:&quot;f5d92ed4-d3b2-45d9-b2d2-e3cb94b77610&quot;}" hidden="1"/>
+        <xdr:cNvPr id="116" name="worksheetKey" descr="{&quot;key&quot;:&quot;worksheetKey&quot;,&quot;value&quot;:&quot;f5d92ed4-d3b2-45d9-b2d2-e3cb94b77610&quot;}" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000074000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2185,6 +2210,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2220,6 +2262,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2395,47 +2454,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:O39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7:L8"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="2" width="4.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="4.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="58.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="2.6640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="1"/>
     <col min="15" max="15" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="27" customHeight="1">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
@@ -2449,10 +2508,10 @@
         <v>55</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="98" t="s">
+      <c r="G3" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="98"/>
+      <c r="H3" s="108"/>
       <c r="I3" s="5" t="s">
         <v>63</v>
       </c>
@@ -2470,10 +2529,10 @@
       <c r="F4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="98" t="s">
+      <c r="G4" s="108" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="98"/>
+      <c r="H4" s="108"/>
       <c r="I4" s="38" t="s">
         <v>41</v>
       </c>
@@ -2492,35 +2551,35 @@
       <c r="F5" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="98" t="s">
+      <c r="G5" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="98"/>
+      <c r="H5" s="108"/>
       <c r="I5" s="38" t="s">
         <v>24</v>
       </c>
       <c r="J5" s="38"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="2:15" ht="14.25" thickBot="1"/>
+    <row r="6" spans="2:15" ht="14" thickBot="1"/>
     <row r="7" spans="2:15" ht="13.5" customHeight="1">
-      <c r="B7" s="81"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="85" t="s">
+      <c r="B7" s="99"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="80" t="s">
+      <c r="E7" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80" t="s">
+      <c r="F7" s="98"/>
+      <c r="G7" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="80"/>
-      <c r="I7" s="87" t="s">
+      <c r="H7" s="98"/>
+      <c r="I7" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="89" t="s">
+      <c r="J7" s="106" t="s">
         <v>62</v>
       </c>
       <c r="K7" s="8"/>
@@ -2530,9 +2589,9 @@
       <c r="N7" s="67"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="83"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="86"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="104"/>
       <c r="E8" s="13" t="s">
         <v>59</v>
       </c>
@@ -2545,12 +2604,12 @@
       <c r="H8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="88"/>
-      <c r="J8" s="90"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="107"/>
       <c r="K8" s="8"/>
       <c r="L8" s="92"/>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" ht="14">
       <c r="B9" s="51">
         <v>100</v>
       </c>
@@ -2583,7 +2642,7 @@
       </c>
       <c r="O9" s="35"/>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" ht="14">
       <c r="B10" s="51">
         <v>200</v>
       </c>
@@ -2616,7 +2675,7 @@
       </c>
       <c r="O10" s="35"/>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" ht="14">
       <c r="B11" s="51">
         <v>300</v>
       </c>
@@ -2648,7 +2707,7 @@
         <v>4.15214236594506E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" ht="14">
       <c r="B12" s="51">
         <v>400</v>
       </c>
@@ -2681,7 +2740,7 @@
       </c>
       <c r="O12" s="35"/>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" ht="14">
       <c r="B13" s="51">
         <v>500</v>
       </c>
@@ -2743,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="14.25" thickBot="1">
+    <row r="16" spans="2:15" ht="14" thickBot="1">
       <c r="B16" s="11" t="s">
         <v>6</v>
       </c>
@@ -2788,20 +2847,20 @@
       <c r="I18" s="37"/>
     </row>
     <row r="20" spans="2:11" ht="13.5" customHeight="1" thickBot="1">
-      <c r="B20" s="93" t="s">
+      <c r="B20" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="93"/>
+      <c r="C20" s="90"/>
       <c r="I20" s="1" t="s">
         <v>64</v>
       </c>
       <c r="J20" s="70"/>
     </row>
     <row r="21" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="95"/>
+      <c r="C21" s="94"/>
       <c r="D21" s="59">
         <v>0</v>
       </c>
@@ -2814,10 +2873,10 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="97"/>
+      <c r="C22" s="96"/>
       <c r="D22" s="55">
         <v>7833894</v>
       </c>
@@ -2830,10 +2889,10 @@
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B23" s="96" t="s">
+      <c r="B23" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="97"/>
+      <c r="C23" s="96"/>
       <c r="D23" s="55">
         <v>0</v>
       </c>
@@ -2844,11 +2903,11 @@
         <v>-7833894</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B24" s="103" t="s">
+    <row r="24" spans="2:11" ht="15" thickBot="1">
+      <c r="B24" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="104"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="62">
         <v>-7833894</v>
       </c>
@@ -2860,29 +2919,29 @@
       </c>
       <c r="K24" s="69"/>
     </row>
-    <row r="27" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B27" s="93" t="s">
+    <row r="27" spans="2:11" ht="14" thickBot="1">
+      <c r="B27" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="93"/>
-      <c r="D27" s="93"/>
-      <c r="E27" s="93"/>
-      <c r="F27" s="93"/>
-    </row>
-    <row r="28" spans="2:11" ht="40.5">
-      <c r="B28" s="105"/>
-      <c r="C28" s="106"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+    </row>
+    <row r="28" spans="2:11" ht="28">
+      <c r="B28" s="86"/>
+      <c r="C28" s="87"/>
       <c r="D28" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="87" t="s">
+      <c r="E28" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87" t="s">
+      <c r="F28" s="79"/>
+      <c r="G28" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="H28" s="99"/>
+      <c r="H28" s="80"/>
       <c r="I28" s="73" t="s">
         <v>49</v>
       </c>
@@ -2890,16 +2949,16 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B29" s="107" t="s">
+    <row r="29" spans="2:11" ht="14" thickBot="1">
+      <c r="B29" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="108"/>
+      <c r="C29" s="89"/>
       <c r="D29" s="16"/>
-      <c r="E29" s="100"/>
-      <c r="F29" s="100"/>
-      <c r="G29" s="100"/>
-      <c r="H29" s="100"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81"/>
       <c r="I29" s="18">
         <f>E29 - D29</f>
         <v>0</v>
@@ -2909,16 +2968,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="14.25" thickBot="1">
+    <row r="30" spans="2:11" ht="15" thickBot="1">
       <c r="G30" s="69"/>
       <c r="I30" s="69"/>
       <c r="J30" s="69"/>
     </row>
-    <row r="31" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B31" s="101" t="s">
+    <row r="31" spans="2:11" ht="14" thickBot="1">
+      <c r="B31" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="102"/>
+      <c r="C31" s="83"/>
       <c r="D31" s="22"/>
       <c r="G31" s="32"/>
     </row>
@@ -2948,20 +3007,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
@@ -2972,6 +3017,20 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <phoneticPr fontId="18"/>
   <printOptions horizontalCentered="1"/>
@@ -2983,7 +3042,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2993,20 +3052,20 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="16.625" customWidth="1"/>
-    <col min="2" max="2" width="61.125" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="39" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="61.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="39" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.625" customWidth="1"/>
-    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="23"/>
     </row>
-    <row r="2" spans="1:6" ht="14.25" thickBot="1">
+    <row r="2" spans="1:6" ht="15" thickBot="1">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -3015,7 +3074,7 @@
       </c>
       <c r="C2" s="68"/>
     </row>
-    <row r="3" spans="1:6" ht="14.25" thickBot="1">
+    <row r="3" spans="1:6" ht="15" thickBot="1">
       <c r="A3" s="75" t="s">
         <v>40</v>
       </c>
@@ -3024,7 +3083,7 @@
       </c>
       <c r="C3" s="68"/>
     </row>
-    <row r="4" spans="1:6" ht="14.25" thickBot="1">
+    <row r="4" spans="1:6" ht="16" thickBot="1">
       <c r="A4" s="76" t="s">
         <v>71</v>
       </c>
@@ -3053,7 +3112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="30">
       <c r="A7" s="65" t="s">
         <v>14</v>
       </c>
@@ -3069,7 +3128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="65" t="s">
         <v>16</v>
       </c>
@@ -3085,7 +3144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="65" t="s">
         <v>18</v>
       </c>
@@ -3101,7 +3160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="15">
       <c r="A10" s="65" t="s">
         <v>20</v>
       </c>
@@ -3117,7 +3176,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="15">
       <c r="A11" s="65" t="s">
         <v>22</v>
       </c>
@@ -3174,267 +3233,277 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+      <selection activeCell="A7" sqref="A7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="43.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.75" customWidth="1"/>
+    <col min="1" max="1" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="101" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25">
-      <c r="A1" s="119" t="s">
+    <row r="1" spans="1:5" ht="20">
+      <c r="A1" s="113" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="121"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="109" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="118"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="111"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="109" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="118"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="111"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="118"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="111"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="109" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="117"/>
-      <c r="C5" s="117"/>
-      <c r="D5" s="117"/>
-      <c r="E5" s="118"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="111"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="109" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="118"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="110"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="111"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="109" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="117"/>
-      <c r="C7" s="117"/>
-      <c r="D7" s="117"/>
-      <c r="E7" s="118"/>
+      <c r="B7" s="110"/>
+      <c r="C7" s="110"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="111"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="113" t="s">
+      <c r="A8" s="116" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="114"/>
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="115"/>
+      <c r="B8" s="117"/>
+      <c r="C8" s="117"/>
+      <c r="D8" s="117"/>
+      <c r="E8" s="118"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="109"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="112"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="109" t="s">
+      <c r="B10" s="112" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="109"/>
-      <c r="D10" s="109"/>
-      <c r="E10" s="109"/>
+      <c r="C10" s="112"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="109" t="s">
+      <c r="B11" s="112" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="109"/>
-      <c r="D11" s="109"/>
-      <c r="E11" s="109"/>
+      <c r="C11" s="112"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="109" t="s">
+      <c r="B12" s="112" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="109"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="112" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="109"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="109"/>
+      <c r="C13" s="112"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="112"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="109" t="s">
+      <c r="B14" s="112" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="109"/>
-      <c r="D14" s="109"/>
-      <c r="E14" s="109"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="112"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="109" t="s">
+      <c r="B15" s="112" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="109"/>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="113" t="s">
+      <c r="A16" s="116" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="114"/>
-      <c r="C16" s="114"/>
-      <c r="D16" s="114"/>
-      <c r="E16" s="115"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="118"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="109" t="s">
+      <c r="B17" s="112" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="109"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="109"/>
+      <c r="C17" s="112"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="112"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="109" t="s">
+      <c r="B18" s="112" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="109"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="109" t="s">
+      <c r="B19" s="112" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="109"/>
-      <c r="D19" s="109"/>
-      <c r="E19" s="109"/>
+      <c r="C19" s="112"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="110" t="s">
+      <c r="B20" s="119" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="111"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="112"/>
+      <c r="C20" s="120"/>
+      <c r="D20" s="120"/>
+      <c r="E20" s="121"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="109" t="s">
+      <c r="B21" s="112" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="109"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="109"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="112"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="109" t="s">
+      <c r="B22" s="112" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="109"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="109"/>
+      <c r="C22" s="112"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="112"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="109" t="s">
+      <c r="B23" s="112" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="109"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="109"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="112"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="109" t="s">
+      <c r="B24" s="112" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
+      <c r="C24" s="112"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="B18:E18"/>
@@ -3446,40 +3515,15 @@
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B17:E17"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008CDC787A71DDF645B3B1EC4B4C087709" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfcc5dabae62faba7569d214b4f3e22c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -3593,17 +3637,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31452BF2-B3C4-4EBE-BE76-B62708FA3B9D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{835BF43D-5F5B-4A92-8B6A-74ACA0EB3617}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3617,17 +3677,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{835BF43D-5F5B-4A92-8B6A-74ACA0EB3617}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31452BF2-B3C4-4EBE-BE76-B62708FA3B9D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>